<commit_message>
Status Report Semana 2
</commit_message>
<xml_diff>
--- a/Docs/Status Report.xlsx
+++ b/Docs/Status Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecdb96fa935d29c7/Área de Trabalho/SPTECH/Pesquisa e Inovação lll/Safe Food/safe-food-docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecdb96fa935d29c7/Área de Trabalho/SPTECH/Pesquisa e Inovação lll/Safe Food/safe-food-docs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="321" documentId="8_{3FB52A1C-E0CE-4D6D-B7A8-6D249B2C0C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22124477-5460-4492-B32D-5D293B195C3B}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="8_{3FB52A1C-E0CE-4D6D-B7A8-6D249B2C0C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AAC2EFF-4C13-4E80-A0C2-6604B772966A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{B3CDE353-4695-40EF-8232-0959744B88AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{B3CDE353-4695-40EF-8232-0959744B88AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="112">
   <si>
     <t>Progressos (Atividades Finalizadas) com seu responsável</t>
   </si>
@@ -214,9 +214,6 @@
     <t>SEMANA XX - DD/MM à DD/MM</t>
   </si>
   <si>
-    <t>SEMANA 2 - 27/03 à 02/03</t>
-  </si>
-  <si>
     <t>Componentes Dots indicador</t>
   </si>
   <si>
@@ -242,6 +239,147 @@
   </si>
   <si>
     <t>Template Status Report</t>
+  </si>
+  <si>
+    <t>Componetes Chips</t>
+  </si>
+  <si>
+    <t>Adicionar Documentação com Swagger</t>
+  </si>
+  <si>
+    <t>Vini</t>
+  </si>
+  <si>
+    <t>Service Signup Estabelecimento</t>
+  </si>
+  <si>
+    <t>Delfino e Vini</t>
+  </si>
+  <si>
+    <t>Home/Dashboard Estabelecimento</t>
+  </si>
+  <si>
+    <t>Protótipo Perfil Estabelecimento</t>
+  </si>
+  <si>
+    <t>React Router Config</t>
+  </si>
+  <si>
+    <t>Componentes Toggle</t>
+  </si>
+  <si>
+    <t>Protótipo FAQ</t>
+  </si>
+  <si>
+    <t>Protótipo Termos de Uso</t>
+  </si>
+  <si>
+    <t>Protótipo Resetar Senha</t>
+  </si>
+  <si>
+    <t>Componente ColGroup</t>
+  </si>
+  <si>
+    <t>Componetes Box</t>
+  </si>
+  <si>
+    <t>Protótipo Cadastro Estabelecimento</t>
+  </si>
+  <si>
+    <t>Protótipo  Perfil Consumidor</t>
+  </si>
+  <si>
+    <t>Protótipo Cadastro Consumidor</t>
+  </si>
+  <si>
+    <t>Protótipo PDP</t>
+  </si>
+  <si>
+    <t>Componente Banner Divulgação Mobile</t>
+  </si>
+  <si>
+    <t>Service Login Estabelecimento</t>
+  </si>
+  <si>
+    <t>Service Login Consumidor</t>
+  </si>
+  <si>
+    <t>Integração JPA SQL Server</t>
+  </si>
+  <si>
+    <t>Script Banco de Dados</t>
+  </si>
+  <si>
+    <t>Conta da cloud criada</t>
+  </si>
+  <si>
+    <t>Value Object Password</t>
+  </si>
+  <si>
+    <t>Protótipo Modal de Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrasos na entrega de alguns itens
+Comunicação fraca
+</t>
+  </si>
+  <si>
+    <t>Componente de Alerta</t>
+  </si>
+  <si>
+    <t>Dominio de Classe do Estabelecimento</t>
+  </si>
+  <si>
+    <t>Service Signup Consumer</t>
+  </si>
+  <si>
+    <t>Dominio de Classe do Consumidor</t>
+  </si>
+  <si>
+    <t>Componente Side Navbar</t>
+  </si>
+  <si>
+    <t>Texto "Sobre Nós"</t>
+  </si>
+  <si>
+    <t>Componente Dots Indicador</t>
+  </si>
+  <si>
+    <t>Componente Modal</t>
+  </si>
+  <si>
+    <t>Componete Checkbox</t>
+  </si>
+  <si>
+    <t>SEMANA 2 - 27/03 à 02/04</t>
+  </si>
+  <si>
+    <t>Http Client Axios React</t>
+  </si>
+  <si>
+    <t>Login Screen</t>
+  </si>
+  <si>
+    <t>Page Cadastro Estabelecimento</t>
+  </si>
+  <si>
+    <t>Page Cadastro Consumidor</t>
+  </si>
+  <si>
+    <t>Componente Comentários</t>
+  </si>
+  <si>
+    <t>Service Create Produt</t>
+  </si>
+  <si>
+    <t>Dominio Produto</t>
+  </si>
+  <si>
+    <t>Delfino, Nakamura
+e Vini</t>
+  </si>
+  <si>
+    <t>Remodelar o DER para Nova Regra de Negócio</t>
   </si>
 </sst>
 </file>
@@ -330,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -828,12 +966,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -881,50 +1063,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,15 +1082,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -965,6 +1105,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -974,6 +1120,72 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -983,34 +1195,52 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1688,21 +1918,21 @@
   <sheetData>
     <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1721,17 +1951,17 @@
     </row>
     <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="45" t="s">
+      <c r="C12" s="32"/>
+      <c r="E12" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
@@ -1740,169 +1970,154 @@
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="13"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="25"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="B27:G27"/>
@@ -1913,6 +2128,21 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1927,7 +2157,7 @@
   </sheetPr>
   <dimension ref="B8:I55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1944,50 +2174,50 @@
   <sheetData>
     <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="E10" s="60" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="E10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="48" t="s">
+      <c r="C12" s="32"/>
+      <c r="E12" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="50"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
@@ -1996,13 +2226,13 @@
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
@@ -2011,11 +2241,11 @@
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
@@ -2024,11 +2254,11 @@
       <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
@@ -2037,11 +2267,11 @@
       <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="53"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
@@ -2050,11 +2280,11 @@
       <c r="C17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
@@ -2063,11 +2293,11 @@
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="53"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
@@ -2076,11 +2306,11 @@
       <c r="C19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="53"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
@@ -2089,24 +2319,24 @@
       <c r="C20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="53"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
@@ -2180,11 +2410,11 @@
       <c r="C27" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="53"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
@@ -2279,7 +2509,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>25</v>
@@ -2349,229 +2579,219 @@
       <c r="C40" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="54"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="56"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="57"/>
     </row>
     <row r="41" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="42" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="28"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="32"/>
     </row>
     <row r="43" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="29" t="s">
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I43" s="31"/>
+      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="23" t="s">
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="25"/>
+      <c r="I44" s="51"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="20" t="s">
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="22"/>
+      <c r="I45" s="48"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="20" t="s">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="22"/>
+      <c r="I46" s="48"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="20" t="s">
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I47" s="22"/>
+      <c r="I47" s="48"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="20" t="s">
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I48" s="22"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="20" t="s">
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="I49" s="22"/>
+      <c r="I49" s="48"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="20" t="s">
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="I50" s="22"/>
+      <c r="I50" s="48"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="20" t="s">
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I51" s="22"/>
+      <c r="I51" s="48"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" s="48"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B53" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="20" t="s">
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="22"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B53" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="22"/>
+      <c r="I53" s="48"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B54" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="20" t="s">
+      <c r="B54" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="I54" s="22"/>
+      <c r="I54" s="48"/>
     </row>
     <row r="55" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="17" t="s">
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="I55" s="19"/>
+      <c r="I55" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E9:I9"/>
     <mergeCell ref="B42:I42"/>
     <mergeCell ref="B43:G43"/>
     <mergeCell ref="H43:I43"/>
@@ -2584,16 +2804,26 @@
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="H54:I54"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2603,10 +2833,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE75F18-1C55-4DC2-8188-F9607B4C70B7}">
-  <dimension ref="B8:I28"/>
+  <dimension ref="B8:I58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58:I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2622,50 +2852,50 @@
   <sheetData>
     <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
+      <c r="B9" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="E10" s="8" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="E10" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="45" t="s">
+      <c r="C12" s="32"/>
+      <c r="E12" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
@@ -2674,151 +2904,873 @@
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="E13" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="65"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="67"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="65"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="65"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B22" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="65"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="65"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B26" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="65"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="67"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="67"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="67"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B30" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="65"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="67"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B31" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="65"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="67"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B32" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="65"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="67"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="65"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B36" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="65"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B37" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="65"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67"/>
+    </row>
+    <row r="38" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="68"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="70"/>
+    </row>
+    <row r="39" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="32"/>
+    </row>
+    <row r="41" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="39"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B42" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="51"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B43" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="48"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B44" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="48"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B45" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="48"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B46" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="48"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B47" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="48"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B48" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I48" s="48"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="48"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B50" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" s="48"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B51" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="48"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B52" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" s="48"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B53" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" s="48"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B54" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="I54" s="48"/>
+    </row>
+    <row r="55" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="I55" s="73"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B56" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="I56" s="48"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B57" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="I57" s="48"/>
+    </row>
+    <row r="58" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I58" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="42">
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="E13:I38"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:I12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E6321D-8556-4CCB-A294-54382012FCAF}">
+  <dimension ref="B8:I28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="61.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.36328125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="9.90625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="E10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="E12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="13"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="25"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -2854,259 +3806,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E6321D-8556-4CCB-A294-54382012FCAF}">
-  <dimension ref="B8:I28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="61.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" style="1" customWidth="1"/>
-    <col min="5" max="8" width="8.7265625" style="1"/>
-    <col min="9" max="9" width="9.90625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-    </row>
-    <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-    </row>
-    <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="4"/>
-      <c r="C14" s="13"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="4"/>
-      <c r="C15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="4"/>
-      <c r="C17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B18" s="4"/>
-      <c r="C18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B19" s="4"/>
-      <c r="C19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
-    </row>
-    <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="7"/>
-      <c r="C20" s="16"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-    </row>
-    <row r="23" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="31"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="25"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
-    </row>
-    <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3D7A97-D8F2-4975-826A-68E102434B63}">
   <dimension ref="B8:I28"/>
@@ -3128,21 +3827,21 @@
   <sheetData>
     <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
+      <c r="B9" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
@@ -3161,17 +3860,17 @@
     </row>
     <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="45" t="s">
+      <c r="C12" s="32"/>
+      <c r="E12" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
@@ -3180,165 +3879,160 @@
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="13"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="25"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="E15:I15"/>
@@ -3347,12 +4041,17 @@
     <mergeCell ref="E18:I18"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H28:I28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3381,21 +4080,21 @@
   <sheetData>
     <row r="8" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:9" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="E9" s="42" t="s">
+      <c r="B9" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="E9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
@@ -3414,17 +4113,17 @@
     </row>
     <row r="11" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="E12" s="45" t="s">
+      <c r="C12" s="32"/>
+      <c r="E12" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11" t="s">
@@ -3433,165 +4132,160 @@
       <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="34"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="4"/>
       <c r="C14" s="13"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="34"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="14"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="14"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="14"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="14"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="34"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="29" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="25"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="51"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="48"/>
     </row>
     <row r="28" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="E15:I15"/>
@@ -3600,12 +4294,17 @@
     <mergeCell ref="E18:I18"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="H28:I28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>